<commit_message>
viz: add safety accuracy heatmaps; excel: conditional formatting for pivot & safety sheets
</commit_message>
<xml_diff>
--- a/exports/metrics.xlsx
+++ b/exports/metrics.xlsx
@@ -2262,9 +2262,6 @@
       <c r="G20" t="n">
         <v>1500</v>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
         <v>1</v>
       </c>
@@ -2346,9 +2343,6 @@
       <c r="G21" t="n">
         <v>1000</v>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>1</v>
       </c>
@@ -2430,9 +2424,6 @@
       <c r="G22" t="n">
         <v>1000</v>
       </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
         <v>0</v>
       </c>
@@ -2514,9 +2505,6 @@
       <c r="G23" t="n">
         <v>1500</v>
       </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
         <v>1</v>
       </c>
@@ -2598,9 +2586,6 @@
       <c r="G24" t="n">
         <v>1000</v>
       </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
         <v>1</v>
       </c>
@@ -2682,9 +2667,6 @@
       <c r="G25" t="n">
         <v>1000</v>
       </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
         <v>0.74</v>
       </c>
@@ -2824,6 +2806,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:D4">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FFF5F0"/>
+        <color rgb="00FDBE85"/>
+        <color rgb="00D94801"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2907,6 +2901,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:D4">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FFF5F0"/>
+        <color rgb="00FDBE85"/>
+        <color rgb="00D94801"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2962,6 +2968,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:D2">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FFF5F0"/>
+        <color rgb="00FDBE85"/>
+        <color rgb="00D94801"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3017,6 +3035,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:D2">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FFF5F0"/>
+        <color rgb="00FDBE85"/>
+        <color rgb="00D94801"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3347,6 +3377,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:I9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FFF5F0"/>
+        <color rgb="00FDBE85"/>
+        <color rgb="00D94801"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>